<commit_message>
Added word document generation
Payslip generation now also generates a word document
</commit_message>
<xml_diff>
--- a/payslips.xlsx
+++ b/payslips.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,25 +492,25 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1100</v>
+        <v>1234</v>
       </c>
       <c r="D2" t="n">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="E2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" t="n">
         <v>5</v>
       </c>
-      <c r="F2" t="n">
-        <v>4</v>
-      </c>
       <c r="G2" t="n">
-        <v>5500</v>
+        <v>3702</v>
       </c>
       <c r="H2" t="n">
-        <v>400</v>
+        <v>615</v>
       </c>
       <c r="I2" t="n">
-        <v>5900</v>
+        <v>4317</v>
       </c>
     </row>
     <row r="3">
@@ -525,25 +525,25 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1200</v>
+        <v>2345</v>
       </c>
       <c r="D3" t="n">
-        <v>100</v>
+        <v>234</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>4800</v>
+        <v>4690</v>
       </c>
       <c r="H3" t="n">
-        <v>200</v>
+        <v>234</v>
       </c>
       <c r="I3" t="n">
-        <v>5000</v>
+        <v>4924</v>
       </c>
     </row>
     <row r="4">
@@ -558,157 +558,25 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2000</v>
+        <v>1234</v>
       </c>
       <c r="D4" t="n">
-        <v>200</v>
+        <v>123</v>
       </c>
       <c r="E4" t="n">
         <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4" t="n">
-        <v>6000</v>
+        <v>3702</v>
       </c>
       <c r="H4" t="n">
-        <v>1000</v>
+        <v>492</v>
       </c>
       <c r="I4" t="n">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>SNAKE</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>SOLID</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D5" t="n">
-        <v>150</v>
-      </c>
-      <c r="E5" t="n">
-        <v>5</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" t="n">
-        <v>7500</v>
-      </c>
-      <c r="H5" t="n">
-        <v>150</v>
-      </c>
-      <c r="I5" t="n">
-        <v>7650</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>SNAKE</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>LIQUID</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1400</v>
-      </c>
-      <c r="D6" t="n">
-        <v>120</v>
-      </c>
-      <c r="E6" t="n">
-        <v>6</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>8400</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>8400</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>SNAKE</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SOLIDUS</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1700</v>
-      </c>
-      <c r="D7" t="n">
-        <v>140</v>
-      </c>
-      <c r="E7" t="n">
-        <v>3</v>
-      </c>
-      <c r="F7" t="n">
-        <v>7</v>
-      </c>
-      <c r="G7" t="n">
-        <v>5100</v>
-      </c>
-      <c r="H7" t="n">
-        <v>980</v>
-      </c>
-      <c r="I7" t="n">
-        <v>6080</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>SNAKE</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>NAKED</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>1300</v>
-      </c>
-      <c r="D8" t="n">
-        <v>100</v>
-      </c>
-      <c r="E8" t="n">
-        <v>3</v>
-      </c>
-      <c r="F8" t="n">
-        <v>10</v>
-      </c>
-      <c r="G8" t="n">
-        <v>3900</v>
-      </c>
-      <c r="H8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="I8" t="n">
-        <v>4900</v>
+        <v>4194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>